<commit_message>
added GridCal shortcut script
</commit_message>
<xml_diff>
--- a/Grid.xlsx
+++ b/Grid.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="135">
   <si>
     <t>Property</t>
   </si>
@@ -44,7 +44,7 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Grid</t>
+    <t>Bloc energy grid</t>
   </si>
   <si>
     <t>Comments</t>
@@ -113,10 +113,10 @@
     <t>0j</t>
   </si>
   <si>
-    <t>-752.0</t>
-  </si>
-  <si>
-    <t>211.0</t>
+    <t>-1119.0</t>
+  </si>
+  <si>
+    <t>28.0</t>
   </si>
   <si>
     <t>20.0</t>
@@ -134,55 +134,55 @@
     <t>Bloque de pisos</t>
   </si>
   <si>
-    <t>-293.0</t>
-  </si>
-  <si>
-    <t>90.0</t>
+    <t>-660.0</t>
+  </si>
+  <si>
+    <t>-93.0</t>
   </si>
   <si>
     <t>Bus 3</t>
   </si>
   <si>
-    <t>-890.0</t>
-  </si>
-  <si>
-    <t>-199.0</t>
+    <t>-1257.0</t>
+  </si>
+  <si>
+    <t>-382.0</t>
   </si>
   <si>
     <t>fabrica</t>
   </si>
   <si>
-    <t>-593.0</t>
-  </si>
-  <si>
-    <t>-316.0</t>
+    <t>-960.0</t>
+  </si>
+  <si>
+    <t>-499.0</t>
   </si>
   <si>
     <t>Bus 5</t>
   </si>
   <si>
-    <t>-1040.0</t>
-  </si>
-  <si>
-    <t>55.0</t>
+    <t>-1407.0</t>
+  </si>
+  <si>
+    <t>-128.0</t>
   </si>
   <si>
     <t>Bus 7</t>
   </si>
   <si>
-    <t>-1395.0</t>
-  </si>
-  <si>
-    <t>-88.0</t>
+    <t>-1762.0</t>
+  </si>
+  <si>
+    <t>-271.0</t>
   </si>
   <si>
     <t>compañia</t>
   </si>
   <si>
-    <t>-1270.0</t>
-  </si>
-  <si>
-    <t>253.0</t>
+    <t>-1637.0</t>
+  </si>
+  <si>
+    <t>70.0</t>
   </si>
   <si>
     <t>bus_from</t>
@@ -248,10 +248,7 @@
     <t>0.05</t>
   </si>
   <si>
-    <t>1.0000000000000001e-20</t>
-  </si>
-  <si>
-    <t>1</t>
+    <t>1e-20</t>
   </si>
   <si>
     <t>line</t>
@@ -862,40 +859,40 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="B1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>114</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>115</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -958,16 +955,16 @@
         <v>60</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>127</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -994,25 +991,25 @@
         <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -1520,7 +1517,7 @@
         <v>73</v>
       </c>
       <c r="M2" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="N2" t="s">
         <v>69</v>
@@ -1535,10 +1532,10 @@
         <v>69</v>
       </c>
       <c r="R2" t="s">
+        <v>74</v>
+      </c>
+      <c r="S2" t="s">
         <v>75</v>
-      </c>
-      <c r="S2" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -1579,7 +1576,7 @@
         <v>73</v>
       </c>
       <c r="M3" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="N3" t="s">
         <v>69</v>
@@ -1594,10 +1591,10 @@
         <v>69</v>
       </c>
       <c r="R3" t="s">
+        <v>74</v>
+      </c>
+      <c r="S3" t="s">
         <v>75</v>
-      </c>
-      <c r="S3" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -1638,7 +1635,7 @@
         <v>73</v>
       </c>
       <c r="M4" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="N4" t="s">
         <v>69</v>
@@ -1653,10 +1650,10 @@
         <v>69</v>
       </c>
       <c r="R4" t="s">
+        <v>74</v>
+      </c>
+      <c r="S4" t="s">
         <v>75</v>
-      </c>
-      <c r="S4" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -1697,7 +1694,7 @@
         <v>73</v>
       </c>
       <c r="M5" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="N5" t="s">
         <v>69</v>
@@ -1712,10 +1709,10 @@
         <v>69</v>
       </c>
       <c r="R5" t="s">
+        <v>74</v>
+      </c>
+      <c r="S5" t="s">
         <v>75</v>
-      </c>
-      <c r="S5" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:19">
@@ -1756,7 +1753,7 @@
         <v>73</v>
       </c>
       <c r="M6" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="N6" t="s">
         <v>69</v>
@@ -1771,10 +1768,10 @@
         <v>69</v>
       </c>
       <c r="R6" t="s">
+        <v>74</v>
+      </c>
+      <c r="S6" t="s">
         <v>75</v>
-      </c>
-      <c r="S6" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:19">
@@ -1815,7 +1812,7 @@
         <v>73</v>
       </c>
       <c r="M7" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="N7" t="s">
         <v>69</v>
@@ -1830,10 +1827,10 @@
         <v>69</v>
       </c>
       <c r="R7" t="s">
+        <v>74</v>
+      </c>
+      <c r="S7" t="s">
         <v>75</v>
-      </c>
-      <c r="S7" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:19">
@@ -1874,7 +1871,7 @@
         <v>73</v>
       </c>
       <c r="M8" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="N8" t="s">
         <v>69</v>
@@ -1889,10 +1886,10 @@
         <v>69</v>
       </c>
       <c r="R8" t="s">
+        <v>74</v>
+      </c>
+      <c r="S8" t="s">
         <v>75</v>
-      </c>
-      <c r="S8" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:19">
@@ -1933,7 +1930,7 @@
         <v>73</v>
       </c>
       <c r="M9" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="N9" t="s">
         <v>69</v>
@@ -1948,10 +1945,10 @@
         <v>69</v>
       </c>
       <c r="R9" t="s">
+        <v>74</v>
+      </c>
+      <c r="S9" t="s">
         <v>75</v>
-      </c>
-      <c r="S9" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:19">
@@ -1992,7 +1989,7 @@
         <v>73</v>
       </c>
       <c r="M10" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="N10" t="s">
         <v>69</v>
@@ -2007,10 +2004,10 @@
         <v>69</v>
       </c>
       <c r="R10" t="s">
+        <v>74</v>
+      </c>
+      <c r="S10" t="s">
         <v>75</v>
-      </c>
-      <c r="S10" t="s">
-        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -2037,19 +2034,19 @@
         <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>80</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>55</v>
@@ -2063,7 +2060,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C2" t="s">
         <v>34</v>
@@ -2078,7 +2075,7 @@
         <v>27</v>
       </c>
       <c r="G2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
@@ -2092,7 +2089,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C3" t="s">
         <v>37</v>
@@ -2107,7 +2104,7 @@
         <v>27</v>
       </c>
       <c r="G3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
@@ -2121,7 +2118,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C4" t="s">
         <v>40</v>
@@ -2136,7 +2133,7 @@
         <v>27</v>
       </c>
       <c r="G4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
@@ -2150,7 +2147,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C5" t="s">
         <v>43</v>
@@ -2165,7 +2162,7 @@
         <v>27</v>
       </c>
       <c r="G5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
@@ -2179,7 +2176,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C6" t="s">
         <v>46</v>
@@ -2194,7 +2191,7 @@
         <v>27</v>
       </c>
       <c r="G6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H6" t="n">
         <v>0</v>
@@ -2208,7 +2205,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C7" t="s">
         <v>49</v>
@@ -2256,13 +2253,13 @@
         <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>55</v>
@@ -2276,7 +2273,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C2" t="s">
         <v>46</v>
@@ -2285,7 +2282,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
@@ -2318,40 +2315,40 @@
         <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>103</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>55</v>
@@ -2360,19 +2357,19 @@
         <v>56</v>
       </c>
       <c r="Q1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:21">
@@ -2380,7 +2377,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C2" t="s">
         <v>46</v>
@@ -2464,37 +2461,37 @@
         <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>96</v>
-      </c>
       <c r="H1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>103</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>55</v>
@@ -2508,7 +2505,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C2" t="s">
         <v>21</v>
@@ -2574,13 +2571,13 @@
         <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>55</v>
@@ -2594,7 +2591,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C2" t="s">
         <v>40</v>
@@ -2603,7 +2600,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
@@ -2633,16 +2630,16 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="B1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>114</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>115</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>